<commit_message>
uploaded code weather normalization relate
</commit_message>
<xml_diff>
--- a/Code/converter/PMfile/PMoutput/testInput1_temp.xlsx
+++ b/Code/converter/PMfile/PMoutput/testInput1_temp.xlsx
@@ -26,6 +26,12 @@
     <t>Cost ($)</t>
   </si>
   <si>
+    <t>Custom ID</t>
+  </si>
+  <si>
+    <t>Custom Meter ID</t>
+  </si>
+  <si>
     <t>District Hot Water</t>
   </si>
   <si>
@@ -48,12 +54,6 @@
   </si>
   <si>
     <t>OSHER extension</t>
-  </si>
-  <si>
-    <t>Portfolio Manager ID</t>
-  </si>
-  <si>
-    <t>Portfolio Manager Meter ID</t>
   </si>
   <si>
     <t>Potable Indoor</t>
@@ -472,19 +472,19 @@
         <v>14</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s" s="1">
         <v>16</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s" s="1">
         <v>19</v>
@@ -501,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="n">
         <v>4674008</v>
@@ -510,7 +510,7 @@
         <v>16873474</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n" s="2">
         <v>41944.0</v>
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="n">
         <v>4674008</v>
@@ -542,7 +542,7 @@
         <v>16873474</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n" s="2">
         <v>41974.0</v>
@@ -565,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
         <v>4674008</v>
@@ -574,7 +574,7 @@
         <v>16873474</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n" s="2">
         <v>42005.0</v>
@@ -597,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
         <v>4674008</v>
@@ -606,7 +606,7 @@
         <v>16873474</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5" t="n" s="2">
         <v>42036.0</v>
@@ -629,7 +629,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="n">
         <v>4674008</v>
@@ -638,7 +638,7 @@
         <v>16873474</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n" s="2">
         <v>42064.0</v>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
         <v>4674008</v>
@@ -670,7 +670,7 @@
         <v>16873474</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F7" t="n" s="2">
         <v>42095.0</v>
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
         <v>4674008</v>
@@ -702,7 +702,7 @@
         <v>16873474</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n" s="2">
         <v>42125.0</v>
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
         <v>4674008</v>
@@ -734,7 +734,7 @@
         <v>16873474</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F9" t="n" s="2">
         <v>42156.0</v>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" t="n">
         <v>4674008</v>
@@ -766,7 +766,7 @@
         <v>16873474</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F10" t="n" s="2">
         <v>42186.0</v>
@@ -789,7 +789,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C11" t="n">
         <v>4674008</v>
@@ -798,7 +798,7 @@
         <v>16873474</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n" s="2">
         <v>42217.0</v>
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12" t="n">
         <v>4674008</v>
@@ -830,7 +830,7 @@
         <v>16873474</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F12" t="n" s="2">
         <v>42248.0</v>
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" t="n">
         <v>4674008</v>
@@ -862,7 +862,7 @@
         <v>16873474</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n" s="2">
         <v>42278.0</v>
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" t="n">
         <v>4674008</v>
@@ -906,7 +906,7 @@
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J14" t="n">
         <v>8.0</v>
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C15" t="n">
         <v>4674008</v>
@@ -938,7 +938,7 @@
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J15" t="n">
         <v>10.0</v>
@@ -949,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C16" t="n">
         <v>4674008</v>
@@ -970,7 +970,7 @@
         <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J16" t="n">
         <v>12.0</v>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C17" t="n">
         <v>4674008</v>
@@ -1002,7 +1002,7 @@
         <v>7</v>
       </c>
       <c r="I17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J17" t="n">
         <v>14.0</v>
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" t="n">
         <v>4674008</v>
@@ -1034,7 +1034,7 @@
         <v>8</v>
       </c>
       <c r="I18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J18" t="n">
         <v>16.0</v>
@@ -1045,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19" t="n">
         <v>4674008</v>
@@ -1066,7 +1066,7 @@
         <v>9</v>
       </c>
       <c r="I19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J19" t="n">
         <v>18.0</v>
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C20" t="n">
         <v>4674008</v>
@@ -1098,7 +1098,7 @@
         <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J20" t="n">
         <v>20.0</v>
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C21" t="n">
         <v>4674008</v>
@@ -1130,7 +1130,7 @@
         <v>11</v>
       </c>
       <c r="I21" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J21" t="n">
         <v>22.0</v>
@@ -1141,7 +1141,7 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C22" t="n">
         <v>4674008</v>
@@ -1162,7 +1162,7 @@
         <v>12</v>
       </c>
       <c r="I22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J22" t="n">
         <v>24.0</v>
@@ -1173,7 +1173,7 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C23" t="n">
         <v>4674008</v>
@@ -1194,7 +1194,7 @@
         <v>13</v>
       </c>
       <c r="I23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J23" t="n">
         <v>26.0</v>
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C24" t="n">
         <v>4674008</v>
@@ -1226,7 +1226,7 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J24" t="n">
         <v>4.0</v>
@@ -1237,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C25" t="n">
         <v>4674008</v>
@@ -1258,7 +1258,7 @@
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J25" t="n">
         <v>6.0</v>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C26" t="n">
         <v>4674008</v>
@@ -1278,7 +1278,7 @@
         <v>16873475</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F26" t="n" s="2">
         <v>41944.0</v>
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C27" t="n">
         <v>4674008</v>
@@ -1310,7 +1310,7 @@
         <v>16873475</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F27" t="n" s="2">
         <v>41974.0</v>
@@ -1333,7 +1333,7 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C28" t="n">
         <v>4674008</v>
@@ -1342,7 +1342,7 @@
         <v>16873475</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F28" t="n" s="2">
         <v>42005.0</v>
@@ -1365,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C29" t="n">
         <v>4674008</v>
@@ -1374,7 +1374,7 @@
         <v>16873475</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F29" t="n" s="2">
         <v>42036.0</v>
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C30" t="n">
         <v>4674008</v>
@@ -1406,7 +1406,7 @@
         <v>16873475</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F30" t="n" s="2">
         <v>42064.0</v>
@@ -1429,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C31" t="n">
         <v>4674008</v>
@@ -1438,7 +1438,7 @@
         <v>16873475</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F31" t="n" s="2">
         <v>42095.0</v>
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C32" t="n">
         <v>4674008</v>
@@ -1470,7 +1470,7 @@
         <v>16873475</v>
       </c>
       <c r="E32" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F32" t="n" s="2">
         <v>42125.0</v>
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C33" t="n">
         <v>4674008</v>
@@ -1502,7 +1502,7 @@
         <v>16873475</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F33" t="n" s="2">
         <v>42156.0</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C34" t="n">
         <v>4674008</v>
@@ -1534,7 +1534,7 @@
         <v>16873475</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F34" t="n" s="2">
         <v>42186.0</v>
@@ -1557,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C35" t="n">
         <v>4674008</v>
@@ -1566,7 +1566,7 @@
         <v>16873475</v>
       </c>
       <c r="E35" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F35" t="n" s="2">
         <v>42217.0</v>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C36" t="n">
         <v>4674008</v>
@@ -1598,7 +1598,7 @@
         <v>16873475</v>
       </c>
       <c r="E36" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F36" t="n" s="2">
         <v>42248.0</v>
@@ -1621,7 +1621,7 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C37" t="n">
         <v>4674008</v>
@@ -1630,7 +1630,7 @@
         <v>16873475</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F37" t="n" s="2">
         <v>42278.0</v>
@@ -1653,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C38" t="n">
         <v>4674008</v>
@@ -1662,7 +1662,7 @@
         <v>16873476</v>
       </c>
       <c r="E38" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n" s="2">
         <v>41944.0</v>
@@ -1685,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C39" t="n">
         <v>4674008</v>
@@ -1694,7 +1694,7 @@
         <v>16873476</v>
       </c>
       <c r="E39" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n" s="2">
         <v>41974.0</v>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C40" t="n">
         <v>4674008</v>
@@ -1726,7 +1726,7 @@
         <v>16873476</v>
       </c>
       <c r="E40" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n" s="2">
         <v>42005.0</v>
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C41" t="n">
         <v>4674008</v>
@@ -1758,7 +1758,7 @@
         <v>16873476</v>
       </c>
       <c r="E41" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n" s="2">
         <v>42036.0</v>
@@ -1781,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C42" t="n">
         <v>4674008</v>
@@ -1790,7 +1790,7 @@
         <v>16873476</v>
       </c>
       <c r="E42" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n" s="2">
         <v>42064.0</v>
@@ -1813,7 +1813,7 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C43" t="n">
         <v>4674008</v>
@@ -1822,7 +1822,7 @@
         <v>16873476</v>
       </c>
       <c r="E43" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n" s="2">
         <v>42095.0</v>
@@ -1845,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C44" t="n">
         <v>4674008</v>
@@ -1854,7 +1854,7 @@
         <v>16873476</v>
       </c>
       <c r="E44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n" s="2">
         <v>42125.0</v>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C45" t="n">
         <v>4674008</v>
@@ -1886,7 +1886,7 @@
         <v>16873476</v>
       </c>
       <c r="E45" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n" s="2">
         <v>42156.0</v>
@@ -1909,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C46" t="n">
         <v>4674008</v>
@@ -1918,7 +1918,7 @@
         <v>16873476</v>
       </c>
       <c r="E46" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n" s="2">
         <v>42186.0</v>
@@ -1941,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C47" t="n">
         <v>4674008</v>
@@ -1950,7 +1950,7 @@
         <v>16873476</v>
       </c>
       <c r="E47" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n" s="2">
         <v>42217.0</v>
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C48" t="n">
         <v>4674008</v>
@@ -1982,7 +1982,7 @@
         <v>16873476</v>
       </c>
       <c r="E48" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n" s="2">
         <v>42248.0</v>
@@ -2005,7 +2005,7 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C49" t="n">
         <v>4674008</v>
@@ -2014,7 +2014,7 @@
         <v>16873476</v>
       </c>
       <c r="E49" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n" s="2">
         <v>42278.0</v>
@@ -2037,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C50" t="n">
         <v>4674008</v>
@@ -2058,7 +2058,7 @@
         <v>4</v>
       </c>
       <c r="I50" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J50" t="n">
         <v>8.0</v>
@@ -2069,7 +2069,7 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C51" t="n">
         <v>4674008</v>
@@ -2090,7 +2090,7 @@
         <v>5</v>
       </c>
       <c r="I51" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J51" t="n">
         <v>10.0</v>
@@ -2101,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C52" t="n">
         <v>4674008</v>
@@ -2122,7 +2122,7 @@
         <v>6</v>
       </c>
       <c r="I52" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J52" t="n">
         <v>12.0</v>
@@ -2133,7 +2133,7 @@
         <v>0</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C53" t="n">
         <v>4674008</v>
@@ -2154,7 +2154,7 @@
         <v>7</v>
       </c>
       <c r="I53" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J53" t="n">
         <v>14.0</v>
@@ -2165,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C54" t="n">
         <v>4674008</v>
@@ -2186,7 +2186,7 @@
         <v>8</v>
       </c>
       <c r="I54" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J54" t="n">
         <v>16.0</v>
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C55" t="n">
         <v>4674008</v>
@@ -2218,7 +2218,7 @@
         <v>9</v>
       </c>
       <c r="I55" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J55" t="n">
         <v>18.0</v>
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C56" t="n">
         <v>4674008</v>
@@ -2250,7 +2250,7 @@
         <v>10</v>
       </c>
       <c r="I56" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J56" t="n">
         <v>20.0</v>
@@ -2261,7 +2261,7 @@
         <v>0</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C57" t="n">
         <v>4674008</v>
@@ -2282,7 +2282,7 @@
         <v>11</v>
       </c>
       <c r="I57" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J57" t="n">
         <v>22.0</v>
@@ -2293,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C58" t="n">
         <v>4674008</v>
@@ -2314,7 +2314,7 @@
         <v>12</v>
       </c>
       <c r="I58" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J58" t="n">
         <v>24.0</v>
@@ -2325,7 +2325,7 @@
         <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C59" t="n">
         <v>4674008</v>
@@ -2346,7 +2346,7 @@
         <v>13</v>
       </c>
       <c r="I59" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J59" t="n">
         <v>26.0</v>
@@ -2357,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C60" t="n">
         <v>4674008</v>
@@ -2378,7 +2378,7 @@
         <v>2</v>
       </c>
       <c r="I60" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J60" t="n">
         <v>4.0</v>
@@ -2389,7 +2389,7 @@
         <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C61" t="n">
         <v>4674008</v>
@@ -2410,7 +2410,7 @@
         <v>3</v>
       </c>
       <c r="I61" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J61" t="n">
         <v>6.0</v>
@@ -2421,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C62" t="n">
         <v>4674008</v>
@@ -2430,7 +2430,7 @@
         <v>16873478</v>
       </c>
       <c r="E62" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n" s="2">
         <v>41944.0</v>
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C63" t="n">
         <v>4674008</v>
@@ -2462,7 +2462,7 @@
         <v>16873478</v>
       </c>
       <c r="E63" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n" s="2">
         <v>41974.0</v>
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C64" t="n">
         <v>4674008</v>
@@ -2494,7 +2494,7 @@
         <v>16873478</v>
       </c>
       <c r="E64" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n" s="2">
         <v>42005.0</v>
@@ -2517,7 +2517,7 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C65" t="n">
         <v>4674008</v>
@@ -2526,7 +2526,7 @@
         <v>16873478</v>
       </c>
       <c r="E65" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n" s="2">
         <v>42036.0</v>
@@ -2549,7 +2549,7 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C66" t="n">
         <v>4674008</v>
@@ -2558,7 +2558,7 @@
         <v>16873478</v>
       </c>
       <c r="E66" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n" s="2">
         <v>42064.0</v>
@@ -2581,7 +2581,7 @@
         <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C67" t="n">
         <v>4674008</v>
@@ -2590,7 +2590,7 @@
         <v>16873478</v>
       </c>
       <c r="E67" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n" s="2">
         <v>42095.0</v>
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C68" t="n">
         <v>4674008</v>
@@ -2622,7 +2622,7 @@
         <v>16873478</v>
       </c>
       <c r="E68" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n" s="2">
         <v>42125.0</v>
@@ -2645,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C69" t="n">
         <v>4674008</v>
@@ -2654,7 +2654,7 @@
         <v>16873478</v>
       </c>
       <c r="E69" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n" s="2">
         <v>42156.0</v>
@@ -2677,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C70" t="n">
         <v>4674008</v>
@@ -2686,7 +2686,7 @@
         <v>16873478</v>
       </c>
       <c r="E70" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n" s="2">
         <v>42186.0</v>
@@ -2709,7 +2709,7 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C71" t="n">
         <v>4674008</v>
@@ -2718,7 +2718,7 @@
         <v>16873478</v>
       </c>
       <c r="E71" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n" s="2">
         <v>42217.0</v>
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C72" t="n">
         <v>4674008</v>
@@ -2750,7 +2750,7 @@
         <v>16873478</v>
       </c>
       <c r="E72" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n" s="2">
         <v>42248.0</v>
@@ -2773,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C73" t="n">
         <v>4674008</v>
@@ -2782,7 +2782,7 @@
         <v>16873478</v>
       </c>
       <c r="E73" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n" s="2">
         <v>42278.0</v>
@@ -2805,7 +2805,7 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C74" t="n">
         <v>4674008</v>
@@ -2814,7 +2814,7 @@
         <v>16873477</v>
       </c>
       <c r="E74" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n" s="2">
         <v>41944.0</v>
@@ -2837,7 +2837,7 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C75" t="n">
         <v>4674008</v>
@@ -2846,7 +2846,7 @@
         <v>16873477</v>
       </c>
       <c r="E75" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n" s="2">
         <v>41974.0</v>
@@ -2869,7 +2869,7 @@
         <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C76" t="n">
         <v>4674008</v>
@@ -2878,7 +2878,7 @@
         <v>16873477</v>
       </c>
       <c r="E76" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n" s="2">
         <v>42005.0</v>
@@ -2901,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C77" t="n">
         <v>4674008</v>
@@ -2910,7 +2910,7 @@
         <v>16873477</v>
       </c>
       <c r="E77" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n" s="2">
         <v>42036.0</v>
@@ -2933,7 +2933,7 @@
         <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C78" t="n">
         <v>4674008</v>
@@ -2942,7 +2942,7 @@
         <v>16873477</v>
       </c>
       <c r="E78" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n" s="2">
         <v>42064.0</v>
@@ -2965,7 +2965,7 @@
         <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C79" t="n">
         <v>4674008</v>
@@ -2974,7 +2974,7 @@
         <v>16873477</v>
       </c>
       <c r="E79" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n" s="2">
         <v>42095.0</v>
@@ -2997,7 +2997,7 @@
         <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C80" t="n">
         <v>4674008</v>
@@ -3006,7 +3006,7 @@
         <v>16873477</v>
       </c>
       <c r="E80" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n" s="2">
         <v>42125.0</v>
@@ -3029,7 +3029,7 @@
         <v>0</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C81" t="n">
         <v>4674008</v>
@@ -3038,7 +3038,7 @@
         <v>16873477</v>
       </c>
       <c r="E81" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n" s="2">
         <v>42156.0</v>
@@ -3061,7 +3061,7 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C82" t="n">
         <v>4674008</v>
@@ -3070,7 +3070,7 @@
         <v>16873477</v>
       </c>
       <c r="E82" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n" s="2">
         <v>42186.0</v>
@@ -3093,7 +3093,7 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C83" t="n">
         <v>4674008</v>
@@ -3102,7 +3102,7 @@
         <v>16873477</v>
       </c>
       <c r="E83" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n" s="2">
         <v>42217.0</v>
@@ -3125,7 +3125,7 @@
         <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C84" t="n">
         <v>4674008</v>
@@ -3134,7 +3134,7 @@
         <v>16873477</v>
       </c>
       <c r="E84" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n" s="2">
         <v>42248.0</v>
@@ -3157,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C85" t="n">
         <v>4674008</v>
@@ -3166,7 +3166,7 @@
         <v>16873477</v>
       </c>
       <c r="E85" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n" s="2">
         <v>42278.0</v>
@@ -3189,7 +3189,7 @@
         <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C86" t="n">
         <v>4674008</v>
@@ -3198,7 +3198,7 @@
         <v>16873484</v>
       </c>
       <c r="E86" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n" s="2">
         <v>41944.0</v>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C87" t="n">
         <v>4674008</v>
@@ -3230,7 +3230,7 @@
         <v>16873484</v>
       </c>
       <c r="E87" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n" s="2">
         <v>41974.0</v>
@@ -3253,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C88" t="n">
         <v>4674008</v>
@@ -3262,7 +3262,7 @@
         <v>16873484</v>
       </c>
       <c r="E88" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n" s="2">
         <v>42005.0</v>
@@ -3285,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C89" t="n">
         <v>4674008</v>
@@ -3294,7 +3294,7 @@
         <v>16873484</v>
       </c>
       <c r="E89" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n" s="2">
         <v>42036.0</v>
@@ -3317,7 +3317,7 @@
         <v>0</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C90" t="n">
         <v>4674008</v>
@@ -3326,7 +3326,7 @@
         <v>16873484</v>
       </c>
       <c r="E90" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n" s="2">
         <v>42064.0</v>
@@ -3349,7 +3349,7 @@
         <v>0</v>
       </c>
       <c r="B91" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C91" t="n">
         <v>4674008</v>
@@ -3358,7 +3358,7 @@
         <v>16873484</v>
       </c>
       <c r="E91" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n" s="2">
         <v>42095.0</v>
@@ -3381,7 +3381,7 @@
         <v>0</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C92" t="n">
         <v>4674008</v>
@@ -3390,7 +3390,7 @@
         <v>16873484</v>
       </c>
       <c r="E92" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n" s="2">
         <v>42125.0</v>
@@ -3413,7 +3413,7 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C93" t="n">
         <v>4674008</v>
@@ -3422,7 +3422,7 @@
         <v>16873484</v>
       </c>
       <c r="E93" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n" s="2">
         <v>42156.0</v>
@@ -3445,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C94" t="n">
         <v>4674008</v>
@@ -3454,7 +3454,7 @@
         <v>16873484</v>
       </c>
       <c r="E94" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n" s="2">
         <v>42186.0</v>
@@ -3477,7 +3477,7 @@
         <v>0</v>
       </c>
       <c r="B95" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C95" t="n">
         <v>4674008</v>
@@ -3486,7 +3486,7 @@
         <v>16873484</v>
       </c>
       <c r="E95" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n" s="2">
         <v>42217.0</v>
@@ -3509,7 +3509,7 @@
         <v>0</v>
       </c>
       <c r="B96" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C96" t="n">
         <v>4674008</v>
@@ -3518,7 +3518,7 @@
         <v>16873484</v>
       </c>
       <c r="E96" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n" s="2">
         <v>42248.0</v>
@@ -3541,7 +3541,7 @@
         <v>0</v>
       </c>
       <c r="B97" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C97" t="n">
         <v>4674008</v>
@@ -3550,7 +3550,7 @@
         <v>16873484</v>
       </c>
       <c r="E97" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n" s="2">
         <v>42278.0</v>
@@ -3582,7 +3582,7 @@
         <v>17284494</v>
       </c>
       <c r="E98" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n" s="2">
         <v>41944.0</v>
@@ -3614,7 +3614,7 @@
         <v>17284494</v>
       </c>
       <c r="E99" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n" s="2">
         <v>41974.0</v>
@@ -3646,7 +3646,7 @@
         <v>17284494</v>
       </c>
       <c r="E100" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F100" t="n" s="2">
         <v>42005.0</v>
@@ -3678,7 +3678,7 @@
         <v>17284494</v>
       </c>
       <c r="E101" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F101" t="n" s="2">
         <v>42036.0</v>
@@ -3710,7 +3710,7 @@
         <v>17284494</v>
       </c>
       <c r="E102" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F102" t="n" s="2">
         <v>42064.0</v>
@@ -3742,7 +3742,7 @@
         <v>17284494</v>
       </c>
       <c r="E103" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F103" t="n" s="2">
         <v>42095.0</v>
@@ -3774,7 +3774,7 @@
         <v>17284494</v>
       </c>
       <c r="E104" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F104" t="n" s="2">
         <v>42125.0</v>
@@ -3806,7 +3806,7 @@
         <v>17284494</v>
       </c>
       <c r="E105" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F105" t="n" s="2">
         <v>42156.0</v>
@@ -3838,7 +3838,7 @@
         <v>17284494</v>
       </c>
       <c r="E106" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F106" t="n" s="2">
         <v>42186.0</v>
@@ -3870,7 +3870,7 @@
         <v>17284494</v>
       </c>
       <c r="E107" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F107" t="n" s="2">
         <v>42217.0</v>
@@ -3902,7 +3902,7 @@
         <v>17284494</v>
       </c>
       <c r="E108" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F108" t="n" s="2">
         <v>42248.0</v>
@@ -3934,7 +3934,7 @@
         <v>17284494</v>
       </c>
       <c r="E109" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F109" t="n" s="2">
         <v>42278.0</v>

</xml_diff>